<commit_message>
New two columns added (lessons)
</commit_message>
<xml_diff>
--- a/src/PARNN_2017II.xlsx
+++ b/src/PARNN_2017II.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eslozano\Google Drive\FUND-PROGRAMACION\SolicitarDatosFundamentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eslozano\Google Drive\FUND-PROGRAMACION\SolicitarDatosFundamentos\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>nombre</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Vacio/2/3</t>
+  </si>
+  <si>
+    <t>1er_lecciones</t>
+  </si>
+  <si>
+    <t>Lecciones</t>
   </si>
 </sst>
 </file>
@@ -710,11 +716,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y62"/>
+  <dimension ref="A1:AA62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K3" sqref="K3"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,18 +731,20 @@
     <col min="6" max="6" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="8" customWidth="1"/>
+    <col min="18" max="18" width="14" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -762,58 +770,64 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
@@ -839,58 +853,64 @@
         <v>1</v>
       </c>
       <c r="I2" s="24">
+        <v>10</v>
+      </c>
+      <c r="J2" s="24">
         <v>100</v>
       </c>
-      <c r="J2" s="24">
+      <c r="K2" s="24">
         <v>20</v>
       </c>
-      <c r="K2" s="24">
+      <c r="L2" s="24">
         <v>32</v>
       </c>
-      <c r="L2" s="24">
+      <c r="M2" s="24">
         <v>45</v>
       </c>
-      <c r="M2" s="24">
+      <c r="N2" s="24">
         <v>10</v>
       </c>
-      <c r="N2" s="25">
+      <c r="O2" s="25">
         <v>20</v>
       </c>
-      <c r="O2" s="25">
+      <c r="P2" s="25">
         <v>1</v>
       </c>
-      <c r="P2" s="25">
+      <c r="Q2" s="25">
+        <v>10</v>
+      </c>
+      <c r="R2" s="25">
         <v>100</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="S2" s="25">
         <v>35</v>
       </c>
-      <c r="R2" s="25">
+      <c r="T2" s="25">
         <v>55</v>
       </c>
-      <c r="S2" s="26">
+      <c r="U2" s="26">
         <v>10</v>
       </c>
-      <c r="T2" s="27">
+      <c r="V2" s="27">
         <v>100</v>
       </c>
-      <c r="U2" s="28">
+      <c r="W2" s="28">
         <v>25</v>
       </c>
-      <c r="V2" s="29">
+      <c r="X2" s="29">
         <v>100</v>
       </c>
-      <c r="W2" s="29">
+      <c r="Y2" s="29">
         <v>40</v>
       </c>
-      <c r="X2" s="29">
+      <c r="Z2" s="29">
         <v>50</v>
       </c>
-      <c r="Y2" s="30">
+      <c r="AA2" s="30">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14"/>
@@ -899,8 +919,8 @@
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -910,14 +930,16 @@
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
-      <c r="T3" s="17"/>
+      <c r="T3" s="13"/>
       <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
+      <c r="V3" s="17"/>
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14"/>
@@ -926,8 +948,8 @@
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -937,14 +959,16 @@
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
-      <c r="T4" s="17"/>
+      <c r="T4" s="13"/>
       <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
+      <c r="V4" s="17"/>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
@@ -953,8 +977,8 @@
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -964,14 +988,16 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
-      <c r="T5" s="17"/>
+      <c r="T5" s="13"/>
       <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
+      <c r="V5" s="17"/>
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14"/>
@@ -980,8 +1006,8 @@
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -991,14 +1017,16 @@
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
-      <c r="T6" s="17"/>
+      <c r="T6" s="13"/>
       <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
+      <c r="V6" s="17"/>
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -1007,8 +1035,8 @@
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
@@ -1018,14 +1046,16 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
-      <c r="T7" s="17"/>
+      <c r="T7" s="13"/>
       <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
+      <c r="V7" s="17"/>
       <c r="W7" s="13"/>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
@@ -1034,8 +1064,8 @@
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
@@ -1045,14 +1075,16 @@
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
-      <c r="T8" s="17"/>
+      <c r="T8" s="13"/>
       <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
+      <c r="V8" s="17"/>
       <c r="W8" s="13"/>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -1061,8 +1093,8 @@
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
@@ -1072,14 +1104,16 @@
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
       <c r="S9" s="13"/>
-      <c r="T9" s="17"/>
+      <c r="T9" s="13"/>
       <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
+      <c r="V9" s="17"/>
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -1088,8 +1122,8 @@
       <c r="F10" s="14"/>
       <c r="G10" s="17"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
@@ -1099,14 +1133,16 @@
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
-      <c r="T10" s="17"/>
+      <c r="T10" s="13"/>
       <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
+      <c r="V10" s="17"/>
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -1115,8 +1151,8 @@
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -1126,14 +1162,16 @@
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
       <c r="S11" s="13"/>
-      <c r="T11" s="17"/>
+      <c r="T11" s="13"/>
       <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
+      <c r="V11" s="17"/>
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
@@ -1142,8 +1180,8 @@
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
@@ -1153,14 +1191,16 @@
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
       <c r="S12" s="13"/>
-      <c r="T12" s="17"/>
+      <c r="T12" s="13"/>
       <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
+      <c r="V12" s="17"/>
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -1169,8 +1209,8 @@
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
@@ -1180,14 +1220,16 @@
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
       <c r="S13" s="13"/>
-      <c r="T13" s="17"/>
+      <c r="T13" s="13"/>
       <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
+      <c r="V13" s="17"/>
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
@@ -1196,25 +1238,27 @@
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="17"/>
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
@@ -1223,8 +1267,8 @@
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
@@ -1234,14 +1278,16 @@
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
       <c r="S15" s="13"/>
-      <c r="T15" s="17"/>
+      <c r="T15" s="13"/>
       <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
+      <c r="V15" s="17"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
@@ -1250,8 +1296,8 @@
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
@@ -1261,14 +1307,16 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
-      <c r="T16" s="17"/>
+      <c r="T16" s="13"/>
       <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
+      <c r="V16" s="17"/>
       <c r="W16" s="13"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
@@ -1277,25 +1325,27 @@
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="17"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
       <c r="S17" s="9"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="17"/>
       <c r="W17" s="13"/>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
@@ -1304,25 +1354,27 @@
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
       <c r="S18" s="9"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="17"/>
       <c r="W18" s="13"/>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -1331,8 +1383,8 @@
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
@@ -1342,14 +1394,16 @@
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
       <c r="S19" s="13"/>
-      <c r="T19" s="17"/>
+      <c r="T19" s="13"/>
       <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
+      <c r="V19" s="17"/>
       <c r="W19" s="13"/>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
@@ -1358,8 +1412,8 @@
       <c r="F20" s="16"/>
       <c r="G20" s="17"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1369,14 +1423,16 @@
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13"/>
-      <c r="T20" s="17"/>
+      <c r="T20" s="13"/>
       <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
+      <c r="V20" s="17"/>
       <c r="W20" s="13"/>
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
@@ -1385,8 +1441,8 @@
       <c r="F21" s="16"/>
       <c r="G21" s="17"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="17"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -1396,14 +1452,16 @@
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
       <c r="S21" s="13"/>
-      <c r="T21" s="17"/>
+      <c r="T21" s="13"/>
       <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
+      <c r="V21" s="17"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="14"/>
@@ -1412,8 +1470,8 @@
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="17"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -1423,14 +1481,16 @@
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
       <c r="S22" s="13"/>
-      <c r="T22" s="17"/>
+      <c r="T22" s="13"/>
       <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
+      <c r="V22" s="17"/>
       <c r="W22" s="13"/>
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="14"/>
@@ -1439,8 +1499,8 @@
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="17"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -1450,14 +1510,16 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
-      <c r="T23" s="17"/>
+      <c r="T23" s="13"/>
       <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
+      <c r="V23" s="17"/>
       <c r="W23" s="13"/>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="14"/>
@@ -1466,8 +1528,8 @@
       <c r="F24" s="16"/>
       <c r="G24" s="17"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="17"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
@@ -1477,14 +1539,16 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
       <c r="S24" s="13"/>
-      <c r="T24" s="17"/>
+      <c r="T24" s="13"/>
       <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
+      <c r="V24" s="17"/>
       <c r="W24" s="13"/>
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14"/>
@@ -1493,8 +1557,8 @@
       <c r="F25" s="16"/>
       <c r="G25" s="17"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
@@ -1504,14 +1568,16 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
-      <c r="T25" s="17"/>
+      <c r="T25" s="13"/>
       <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
+      <c r="V25" s="17"/>
       <c r="W25" s="13"/>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14"/>
@@ -1520,8 +1586,8 @@
       <c r="F26" s="16"/>
       <c r="G26" s="17"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="17"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
@@ -1531,14 +1597,16 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
-      <c r="T26" s="17"/>
+      <c r="T26" s="13"/>
       <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
+      <c r="V26" s="17"/>
       <c r="W26" s="13"/>
       <c r="X26" s="13"/>
       <c r="Y26" s="13"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26" s="13"/>
+      <c r="AA26" s="13"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
@@ -1547,8 +1615,8 @@
       <c r="F27" s="16"/>
       <c r="G27" s="17"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="17"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -1558,14 +1626,16 @@
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
-      <c r="T27" s="17"/>
+      <c r="T27" s="13"/>
       <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
+      <c r="V27" s="17"/>
       <c r="W27" s="13"/>
       <c r="X27" s="13"/>
       <c r="Y27" s="13"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14"/>
@@ -1574,8 +1644,8 @@
       <c r="F28" s="16"/>
       <c r="G28" s="17"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="17"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
@@ -1585,14 +1655,16 @@
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
       <c r="S28" s="13"/>
-      <c r="T28" s="17"/>
+      <c r="T28" s="13"/>
       <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
+      <c r="V28" s="17"/>
       <c r="W28" s="13"/>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z28" s="13"/>
+      <c r="AA28" s="13"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="14"/>
@@ -1601,8 +1673,8 @@
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="17"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
@@ -1612,14 +1684,16 @@
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
       <c r="S29" s="13"/>
-      <c r="T29" s="17"/>
+      <c r="T29" s="13"/>
       <c r="U29" s="13"/>
-      <c r="V29" s="13"/>
+      <c r="V29" s="17"/>
       <c r="W29" s="13"/>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="13"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="14"/>
@@ -1628,8 +1702,8 @@
       <c r="F30" s="16"/>
       <c r="G30" s="17"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="17"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
@@ -1639,14 +1713,16 @@
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
-      <c r="T30" s="17"/>
+      <c r="T30" s="13"/>
       <c r="U30" s="13"/>
-      <c r="V30" s="13"/>
+      <c r="V30" s="17"/>
       <c r="W30" s="13"/>
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
@@ -1655,8 +1731,8 @@
       <c r="F31" s="16"/>
       <c r="G31" s="17"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="17"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
@@ -1666,14 +1742,16 @@
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
       <c r="S31" s="13"/>
-      <c r="T31" s="17"/>
+      <c r="T31" s="13"/>
       <c r="U31" s="13"/>
-      <c r="V31" s="13"/>
+      <c r="V31" s="17"/>
       <c r="W31" s="13"/>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
@@ -1682,25 +1760,27 @@
       <c r="F32" s="16"/>
       <c r="G32" s="17"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="17"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
       <c r="P32" s="13"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
       <c r="S32" s="9"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="13"/>
-      <c r="V32" s="13"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="17"/>
       <c r="W32" s="13"/>
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
@@ -1709,8 +1789,8 @@
       <c r="F33" s="16"/>
       <c r="G33" s="17"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="17"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
@@ -1720,14 +1800,16 @@
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
       <c r="S33" s="13"/>
-      <c r="T33" s="17"/>
+      <c r="T33" s="13"/>
       <c r="U33" s="13"/>
-      <c r="V33" s="13"/>
+      <c r="V33" s="17"/>
       <c r="W33" s="13"/>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
@@ -1736,8 +1818,8 @@
       <c r="F34" s="16"/>
       <c r="G34" s="17"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="17"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
@@ -1747,14 +1829,16 @@
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
-      <c r="T34" s="17"/>
+      <c r="T34" s="13"/>
       <c r="U34" s="13"/>
-      <c r="V34" s="13"/>
+      <c r="V34" s="17"/>
       <c r="W34" s="13"/>
       <c r="X34" s="13"/>
       <c r="Y34" s="13"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34" s="13"/>
+      <c r="AA34" s="13"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
@@ -1763,25 +1847,27 @@
       <c r="F35" s="16"/>
       <c r="G35" s="17"/>
       <c r="H35" s="13"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="17"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
       <c r="S35" s="9"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="17"/>
       <c r="W35" s="13"/>
       <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="13"/>
+      <c r="AA35" s="13"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
@@ -1790,25 +1876,27 @@
       <c r="F36" s="16"/>
       <c r="G36" s="17"/>
       <c r="H36" s="13"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="17"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
       <c r="S36" s="9"/>
-      <c r="T36" s="17"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="17"/>
       <c r="W36" s="13"/>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="14"/>
@@ -1817,8 +1905,8 @@
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="17"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
@@ -1828,14 +1916,16 @@
       <c r="Q37" s="13"/>
       <c r="R37" s="13"/>
       <c r="S37" s="13"/>
-      <c r="T37" s="17"/>
+      <c r="T37" s="13"/>
       <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
+      <c r="V37" s="17"/>
       <c r="W37" s="13"/>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37" s="13"/>
+      <c r="AA37" s="13"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
@@ -1844,8 +1934,8 @@
       <c r="F38" s="16"/>
       <c r="G38" s="17"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="17"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
@@ -1855,14 +1945,16 @@
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
       <c r="S38" s="13"/>
-      <c r="T38" s="17"/>
+      <c r="T38" s="13"/>
       <c r="U38" s="13"/>
-      <c r="V38" s="13"/>
+      <c r="V38" s="17"/>
       <c r="W38" s="13"/>
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="14"/>
@@ -1871,25 +1963,27 @@
       <c r="F39" s="16"/>
       <c r="G39" s="17"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="17"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
       <c r="S39" s="9"/>
-      <c r="T39" s="17"/>
-      <c r="U39" s="13"/>
-      <c r="V39" s="13"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="17"/>
       <c r="W39" s="13"/>
       <c r="X39" s="13"/>
       <c r="Y39" s="13"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z39" s="13"/>
+      <c r="AA39" s="13"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
@@ -1898,8 +1992,8 @@
       <c r="F40" s="16"/>
       <c r="G40" s="17"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="17"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
@@ -1909,14 +2003,16 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
-      <c r="T40" s="17"/>
+      <c r="T40" s="13"/>
       <c r="U40" s="13"/>
-      <c r="V40" s="13"/>
+      <c r="V40" s="17"/>
       <c r="W40" s="13"/>
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z40" s="13"/>
+      <c r="AA40" s="13"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="19"/>
@@ -1925,8 +2021,8 @@
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="17"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
       <c r="M41" s="13"/>
@@ -1936,14 +2032,16 @@
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
       <c r="S41" s="13"/>
-      <c r="T41" s="17"/>
+      <c r="T41" s="13"/>
       <c r="U41" s="13"/>
-      <c r="V41" s="13"/>
+      <c r="V41" s="17"/>
       <c r="W41" s="13"/>
       <c r="X41" s="13"/>
       <c r="Y41" s="13"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z41" s="13"/>
+      <c r="AA41" s="13"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
@@ -1952,8 +2050,8 @@
       <c r="F42" s="16"/>
       <c r="G42" s="17"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="17"/>
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
@@ -1963,14 +2061,16 @@
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
       <c r="S42" s="13"/>
-      <c r="T42" s="17"/>
+      <c r="T42" s="13"/>
       <c r="U42" s="13"/>
-      <c r="V42" s="13"/>
+      <c r="V42" s="17"/>
       <c r="W42" s="13"/>
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
@@ -1979,8 +2079,8 @@
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="17"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
       <c r="M43" s="13"/>
@@ -1990,14 +2090,16 @@
       <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
       <c r="S43" s="13"/>
-      <c r="T43" s="17"/>
+      <c r="T43" s="13"/>
       <c r="U43" s="13"/>
-      <c r="V43" s="13"/>
+      <c r="V43" s="17"/>
       <c r="W43" s="13"/>
       <c r="X43" s="13"/>
       <c r="Y43" s="13"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
@@ -2006,8 +2108,8 @@
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
       <c r="H44" s="13"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="17"/>
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
@@ -2017,14 +2119,16 @@
       <c r="Q44" s="13"/>
       <c r="R44" s="13"/>
       <c r="S44" s="13"/>
-      <c r="T44" s="17"/>
+      <c r="T44" s="13"/>
       <c r="U44" s="13"/>
-      <c r="V44" s="13"/>
+      <c r="V44" s="17"/>
       <c r="W44" s="13"/>
       <c r="X44" s="13"/>
       <c r="Y44" s="13"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z44" s="13"/>
+      <c r="AA44" s="13"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
@@ -2033,8 +2137,8 @@
       <c r="F45" s="16"/>
       <c r="G45" s="17"/>
       <c r="H45" s="13"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="17"/>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
@@ -2044,14 +2148,16 @@
       <c r="Q45" s="13"/>
       <c r="R45" s="13"/>
       <c r="S45" s="13"/>
-      <c r="T45" s="17"/>
+      <c r="T45" s="13"/>
       <c r="U45" s="13"/>
-      <c r="V45" s="13"/>
+      <c r="V45" s="17"/>
       <c r="W45" s="13"/>
       <c r="X45" s="13"/>
       <c r="Y45" s="13"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
@@ -2060,8 +2166,8 @@
       <c r="F46" s="16"/>
       <c r="G46" s="17"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="17"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
       <c r="M46" s="13"/>
@@ -2071,14 +2177,16 @@
       <c r="Q46" s="13"/>
       <c r="R46" s="13"/>
       <c r="S46" s="13"/>
-      <c r="T46" s="17"/>
+      <c r="T46" s="13"/>
       <c r="U46" s="13"/>
-      <c r="V46" s="13"/>
+      <c r="V46" s="17"/>
       <c r="W46" s="13"/>
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
@@ -2087,8 +2195,8 @@
       <c r="F47" s="16"/>
       <c r="G47" s="17"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="17"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
       <c r="M47" s="13"/>
@@ -2098,14 +2206,16 @@
       <c r="Q47" s="13"/>
       <c r="R47" s="13"/>
       <c r="S47" s="13"/>
-      <c r="T47" s="17"/>
+      <c r="T47" s="13"/>
       <c r="U47" s="13"/>
-      <c r="V47" s="13"/>
+      <c r="V47" s="17"/>
       <c r="W47" s="13"/>
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
@@ -2114,8 +2224,8 @@
       <c r="F48" s="16"/>
       <c r="G48" s="17"/>
       <c r="H48" s="13"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="17"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
@@ -2125,14 +2235,16 @@
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
       <c r="S48" s="13"/>
-      <c r="T48" s="17"/>
+      <c r="T48" s="13"/>
       <c r="U48" s="13"/>
-      <c r="V48" s="13"/>
+      <c r="V48" s="17"/>
       <c r="W48" s="13"/>
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
@@ -2141,8 +2253,8 @@
       <c r="F49" s="16"/>
       <c r="G49" s="17"/>
       <c r="H49" s="13"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="17"/>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
       <c r="M49" s="13"/>
@@ -2152,14 +2264,16 @@
       <c r="Q49" s="13"/>
       <c r="R49" s="13"/>
       <c r="S49" s="13"/>
-      <c r="T49" s="17"/>
+      <c r="T49" s="13"/>
       <c r="U49" s="13"/>
-      <c r="V49" s="13"/>
+      <c r="V49" s="17"/>
       <c r="W49" s="13"/>
       <c r="X49" s="13"/>
       <c r="Y49" s="13"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
@@ -2168,8 +2282,8 @@
       <c r="F50" s="16"/>
       <c r="G50" s="17"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="17"/>
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
       <c r="M50" s="13"/>
@@ -2179,14 +2293,16 @@
       <c r="Q50" s="13"/>
       <c r="R50" s="13"/>
       <c r="S50" s="13"/>
-      <c r="T50" s="17"/>
+      <c r="T50" s="13"/>
       <c r="U50" s="13"/>
-      <c r="V50" s="13"/>
+      <c r="V50" s="17"/>
       <c r="W50" s="13"/>
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
@@ -2195,8 +2311,8 @@
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
       <c r="H51" s="13"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="17"/>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
       <c r="M51" s="13"/>
@@ -2206,14 +2322,16 @@
       <c r="Q51" s="13"/>
       <c r="R51" s="13"/>
       <c r="S51" s="13"/>
-      <c r="T51" s="17"/>
+      <c r="T51" s="13"/>
       <c r="U51" s="13"/>
-      <c r="V51" s="13"/>
+      <c r="V51" s="17"/>
       <c r="W51" s="13"/>
       <c r="X51" s="13"/>
       <c r="Y51" s="13"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z51" s="13"/>
+      <c r="AA51" s="13"/>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
@@ -2222,8 +2340,8 @@
       <c r="F52" s="16"/>
       <c r="G52" s="17"/>
       <c r="H52" s="13"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="17"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
       <c r="M52" s="13"/>
@@ -2233,14 +2351,16 @@
       <c r="Q52" s="13"/>
       <c r="R52" s="13"/>
       <c r="S52" s="13"/>
-      <c r="T52" s="17"/>
+      <c r="T52" s="13"/>
       <c r="U52" s="13"/>
-      <c r="V52" s="13"/>
+      <c r="V52" s="17"/>
       <c r="W52" s="13"/>
       <c r="X52" s="13"/>
       <c r="Y52" s="13"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z52" s="13"/>
+      <c r="AA52" s="13"/>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -2249,8 +2369,8 @@
       <c r="F53" s="16"/>
       <c r="G53" s="17"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="17"/>
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
       <c r="M53" s="13"/>
@@ -2260,14 +2380,16 @@
       <c r="Q53" s="13"/>
       <c r="R53" s="13"/>
       <c r="S53" s="13"/>
-      <c r="T53" s="20"/>
+      <c r="T53" s="13"/>
       <c r="U53" s="13"/>
-      <c r="V53" s="13"/>
+      <c r="V53" s="20"/>
       <c r="W53" s="13"/>
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z53" s="13"/>
+      <c r="AA53" s="13"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
@@ -2276,8 +2398,8 @@
       <c r="F54" s="16"/>
       <c r="G54" s="17"/>
       <c r="H54" s="13"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="17"/>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
       <c r="M54" s="13"/>
@@ -2287,14 +2409,16 @@
       <c r="Q54" s="13"/>
       <c r="R54" s="13"/>
       <c r="S54" s="13"/>
-      <c r="T54" s="17"/>
+      <c r="T54" s="13"/>
       <c r="U54" s="13"/>
-      <c r="V54" s="13"/>
+      <c r="V54" s="17"/>
       <c r="W54" s="13"/>
       <c r="X54" s="13"/>
       <c r="Y54" s="13"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z54" s="13"/>
+      <c r="AA54" s="13"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
@@ -2303,25 +2427,27 @@
       <c r="F55" s="16"/>
       <c r="G55" s="17"/>
       <c r="H55" s="13"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="17"/>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
       <c r="M55" s="13"/>
       <c r="N55" s="13"/>
       <c r="O55" s="13"/>
       <c r="P55" s="13"/>
-      <c r="Q55" s="9"/>
-      <c r="R55" s="9"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
       <c r="S55" s="9"/>
-      <c r="T55" s="17"/>
-      <c r="U55" s="13"/>
-      <c r="V55" s="13"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="17"/>
       <c r="W55" s="13"/>
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z55" s="13"/>
+      <c r="AA55" s="13"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
@@ -2330,8 +2456,8 @@
       <c r="F56" s="16"/>
       <c r="G56" s="17"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="17"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
       <c r="M56" s="13"/>
@@ -2341,14 +2467,16 @@
       <c r="Q56" s="13"/>
       <c r="R56" s="13"/>
       <c r="S56" s="13"/>
-      <c r="T56" s="17"/>
+      <c r="T56" s="13"/>
       <c r="U56" s="13"/>
-      <c r="V56" s="13"/>
+      <c r="V56" s="17"/>
       <c r="W56" s="13"/>
       <c r="X56" s="13"/>
       <c r="Y56" s="13"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z56" s="13"/>
+      <c r="AA56" s="13"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
@@ -2357,8 +2485,8 @@
       <c r="F57" s="16"/>
       <c r="G57" s="17"/>
       <c r="H57" s="13"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="17"/>
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
       <c r="M57" s="13"/>
@@ -2368,14 +2496,16 @@
       <c r="Q57" s="13"/>
       <c r="R57" s="13"/>
       <c r="S57" s="13"/>
-      <c r="T57" s="17"/>
+      <c r="T57" s="13"/>
       <c r="U57" s="13"/>
-      <c r="V57" s="13"/>
+      <c r="V57" s="17"/>
       <c r="W57" s="13"/>
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z57" s="13"/>
+      <c r="AA57" s="13"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
@@ -2384,8 +2514,8 @@
       <c r="F58" s="16"/>
       <c r="G58" s="17"/>
       <c r="H58" s="13"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="17"/>
       <c r="K58" s="13"/>
       <c r="L58" s="13"/>
       <c r="M58" s="13"/>
@@ -2395,14 +2525,16 @@
       <c r="Q58" s="13"/>
       <c r="R58" s="13"/>
       <c r="S58" s="13"/>
-      <c r="T58" s="17"/>
+      <c r="T58" s="13"/>
       <c r="U58" s="13"/>
-      <c r="V58" s="13"/>
+      <c r="V58" s="17"/>
       <c r="W58" s="13"/>
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z58" s="13"/>
+      <c r="AA58" s="13"/>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -2411,8 +2543,8 @@
       <c r="F59" s="16"/>
       <c r="G59" s="17"/>
       <c r="H59" s="13"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="17"/>
       <c r="K59" s="13"/>
       <c r="L59" s="13"/>
       <c r="M59" s="13"/>
@@ -2422,14 +2554,16 @@
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
       <c r="S59" s="13"/>
-      <c r="T59" s="17"/>
+      <c r="T59" s="13"/>
       <c r="U59" s="13"/>
-      <c r="V59" s="13"/>
+      <c r="V59" s="17"/>
       <c r="W59" s="13"/>
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z59" s="13"/>
+      <c r="AA59" s="13"/>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
@@ -2438,8 +2572,8 @@
       <c r="F60" s="16"/>
       <c r="G60" s="17"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="17"/>
       <c r="K60" s="13"/>
       <c r="L60" s="13"/>
       <c r="M60" s="13"/>
@@ -2449,14 +2583,16 @@
       <c r="Q60" s="13"/>
       <c r="R60" s="13"/>
       <c r="S60" s="13"/>
-      <c r="T60" s="17"/>
+      <c r="T60" s="13"/>
       <c r="U60" s="13"/>
-      <c r="V60" s="13"/>
+      <c r="V60" s="17"/>
       <c r="W60" s="13"/>
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z60" s="13"/>
+      <c r="AA60" s="13"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
@@ -2465,8 +2601,8 @@
       <c r="F61" s="16"/>
       <c r="G61" s="17"/>
       <c r="H61" s="13"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="17"/>
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
       <c r="M61" s="13"/>
@@ -2476,14 +2612,16 @@
       <c r="Q61" s="13"/>
       <c r="R61" s="13"/>
       <c r="S61" s="13"/>
-      <c r="T61" s="17"/>
+      <c r="T61" s="13"/>
       <c r="U61" s="13"/>
-      <c r="V61" s="13"/>
+      <c r="V61" s="17"/>
       <c r="W61" s="13"/>
-      <c r="X61" s="21"/>
+      <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z61" s="21"/>
+      <c r="AA61" s="13"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
@@ -2492,23 +2630,25 @@
       <c r="F62" s="16"/>
       <c r="G62" s="17"/>
       <c r="H62" s="13"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="17"/>
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
       <c r="O62" s="13"/>
       <c r="P62" s="13"/>
-      <c r="Q62" s="9"/>
-      <c r="R62" s="9"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
       <c r="S62" s="9"/>
-      <c r="T62" s="17"/>
-      <c r="U62" s="13"/>
-      <c r="V62" s="13"/>
+      <c r="T62" s="9"/>
+      <c r="U62" s="9"/>
+      <c r="V62" s="17"/>
       <c r="W62" s="13"/>
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
+      <c r="Z62" s="13"/>
+      <c r="AA62" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>